<commit_message>
Menambah system import data customer dan create serta erxport data
</commit_message>
<xml_diff>
--- a/assets/export/Excel_DataPelanggan.xlsx
+++ b/assets/export/Excel_DataPelanggan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\nakasy\assets\export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC5551B-0B5C-4430-B229-50022D54BCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9A7582-4C54-4A7A-9776-6247077CFCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,22 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
-  <si>
-    <t>Kode Customer</t>
-  </si>
-  <si>
-    <t>Phone Customer</t>
-  </si>
-  <si>
-    <t>Nama Customer</t>
-  </si>
-  <si>
-    <t>A22050001</t>
-  </si>
-  <si>
-    <t>Budi Santoso</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t xml:space="preserve"> INSERT DATA CUSTOMER</t>
   </si>
@@ -49,45 +34,15 @@
     <t>Nama Paket</t>
   </si>
   <si>
-    <t>Name_PPPOE</t>
-  </si>
-  <si>
-    <t>Password_PPPOE</t>
-  </si>
-  <si>
-    <t>Alamat Customer</t>
-  </si>
-  <si>
-    <t>Email Customer</t>
-  </si>
-  <si>
     <t>Tanggal Registrasi</t>
   </si>
   <si>
-    <t>Tanggal Terminated</t>
-  </si>
-  <si>
     <t>Nama Area</t>
   </si>
   <si>
     <t>Nama Sales</t>
   </si>
   <si>
-    <t>083134324234</t>
-  </si>
-  <si>
-    <t>budisantoso</t>
-  </si>
-  <si>
-    <t>Home 5</t>
-  </si>
-  <si>
-    <t>Jl. Permata Damai</t>
-  </si>
-  <si>
-    <t>budi@gmail.com</t>
-  </si>
-  <si>
     <t>Keterangan :</t>
   </si>
   <si>
@@ -97,23 +52,197 @@
     <t>data yang di iputkan ke excel harus sama dengan data aplikasi di website dalam penamaan nya (Nama Paket, Nama Area, Nama Sales)</t>
   </si>
   <si>
-    <t>PROB_KBS</t>
-  </si>
-  <si>
-    <t>Alihadi</t>
-  </si>
-  <si>
-    <t>infly</t>
+    <t>Id Paket</t>
+  </si>
+  <si>
+    <t>Id Area</t>
+  </si>
+  <si>
+    <t>Kode Pelanggan</t>
+  </si>
+  <si>
+    <t>Nama Pelanggan</t>
+  </si>
+  <si>
+    <t>Phone Pelanggan</t>
+  </si>
+  <si>
+    <t>ID PPPOE</t>
+  </si>
+  <si>
+    <t>Name PPPOE</t>
+  </si>
+  <si>
+    <t>Password PPPOE</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Id Sales</t>
+  </si>
+  <si>
+    <t>082302052269</t>
+  </si>
+  <si>
+    <t>Home 20</t>
+  </si>
+  <si>
+    <t>*21</t>
+  </si>
+  <si>
+    <t>infly2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JL COKROMINOTO GG LISTRIKAN PERUM GCR NO 42
+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>CKG 050407</t>
+  </si>
+  <si>
+    <t>Dayat</t>
+  </si>
+  <si>
+    <t>081230160585</t>
+  </si>
+  <si>
+    <t>Home 10</t>
+  </si>
+  <si>
+    <t>*2C</t>
+  </si>
+  <si>
+    <t>JL COKROAMINOTO GG LISTRIKAN PERUM GCR NO 22
+KANIGARAN</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>085708290009</t>
+  </si>
+  <si>
+    <t>*27</t>
+  </si>
+  <si>
+    <t>JL COKRO GG LISRIKAN PERUM GRAND CAHAYA RESIDENCE</t>
+  </si>
+  <si>
+    <t>aprinkresna@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-08-21</t>
+  </si>
+  <si>
+    <t>085236790393</t>
+  </si>
+  <si>
+    <t>*20</t>
+  </si>
+  <si>
+    <t>PERUM GCR NO 36	KELURAHAN KANIGARAN</t>
+  </si>
+  <si>
+    <t>f3n1saf1984@gmail.com</t>
+  </si>
+  <si>
+    <t>2023-10-15</t>
+  </si>
+  <si>
+    <t>CKG 050308</t>
+  </si>
+  <si>
+    <t>Siti Nurhayati</t>
+  </si>
+  <si>
+    <t>081222282038</t>
+  </si>
+  <si>
+    <t>Home TV 25</t>
+  </si>
+  <si>
+    <t>*2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JL COKROMINOTO GG LISTRIKAN PERUM GCR NO 14 
+KANIGARAN
+</t>
+  </si>
+  <si>
+    <t>CKG 050408</t>
+  </si>
+  <si>
+    <t>082337882385</t>
+  </si>
+  <si>
+    <t>*24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JL COKROAMINOTO GG LISTRIKAN PERUM GCR NO 15
+KANIGARAN
+</t>
+  </si>
+  <si>
+    <t>Dimas Coba 1</t>
+  </si>
+  <si>
+    <t>Dimas Coba 2</t>
+  </si>
+  <si>
+    <t>Dimas Coba 3</t>
+  </si>
+  <si>
+    <t>Dimas Coba 4</t>
+  </si>
+  <si>
+    <t>Dimas Coba 5</t>
+  </si>
+  <si>
+    <t>Dimas Coba 6</t>
+  </si>
+  <si>
+    <t>coba_dimas01</t>
+  </si>
+  <si>
+    <t>coba_dimas02</t>
+  </si>
+  <si>
+    <t>coba_dimas03</t>
+  </si>
+  <si>
+    <t>coba_dimas04</t>
+  </si>
+  <si>
+    <t>coba_dimas05</t>
+  </si>
+  <si>
+    <t>coba_dimas06</t>
+  </si>
+  <si>
+    <t>Home 30</t>
+  </si>
+  <si>
+    <t>Home 50</t>
+  </si>
+  <si>
+    <t>Free 20 Mbps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,19 +265,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -158,14 +274,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri Bold"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -173,23 +282,19 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -211,53 +316,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -267,8 +369,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,73 +698,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75">
+    <row r="1" spans="1:16" ht="18.75">
       <c r="A1"/>
-      <c r="B1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75">
+    <row r="2" spans="1:16" ht="18.75">
       <c r="A2"/>
-      <c r="B2" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
@@ -671,15 +772,15 @@
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
@@ -695,86 +796,355 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:16" ht="18.75">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="5">
+        <v>7010823005</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="5">
+        <v>3</v>
+      </c>
+      <c r="O6" s="5">
+        <v>176</v>
+      </c>
+      <c r="P6" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="B7" s="5">
+        <v>7010823011</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="5">
+        <v>2</v>
+      </c>
+      <c r="O7" s="5">
+        <v>176</v>
+      </c>
+      <c r="P7" s="5">
         <v>11</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5"/>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
+    <row r="8" spans="1:16" ht="15.75">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B8" s="5">
+        <v>7210823001</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="5">
+        <v>2</v>
+      </c>
+      <c r="O8" s="5">
+        <v>176</v>
+      </c>
+      <c r="P8" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="B9" s="5">
+        <v>7151023001</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2</v>
+      </c>
+      <c r="O9" s="5">
+        <v>95</v>
+      </c>
+      <c r="P9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75">
+      <c r="A10" s="5">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5">
+        <v>7010823004</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="11">
-        <v>44208</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N6"/>
+      <c r="L10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" s="5">
+        <v>11</v>
+      </c>
+      <c r="O10" s="5">
+        <v>177</v>
+      </c>
+      <c r="P10" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75">
+      <c r="A11" s="5">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5">
+        <v>7010823012</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="5">
+        <v>2</v>
+      </c>
+      <c r="O11" s="5">
+        <v>177</v>
+      </c>
+      <c r="P11" s="5">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -783,11 +1153,9 @@
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="H2:N2"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="I6" r:id="rId1" xr:uid="{3CBAB2E2-4A50-4DAC-BEE5-1009A065C688}"/>
-  </hyperlinks>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>